<commit_message>
Added some GUI updates
</commit_message>
<xml_diff>
--- a/Inventory_Management/Avraam/savedInventory_Flammable.xlsx
+++ b/Inventory_Management/Avraam/savedInventory_Flammable.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Description</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>currentNumberOfItemsOnShelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly Spray </t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -101,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -171,6 +177,41 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>1435453.0</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="J2" t="n" s="0">
+        <v>1000.0</v>
+      </c>
+      <c r="K2" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="L2" t="n" s="0">
+        <v>500.0</v>
+      </c>
+      <c r="M2" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="N2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O2" t="n" s="0">
+        <v>20.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>